<commit_message>
Add source to school reopening.
</commit_message>
<xml_diff>
--- a/Data/SchoolReopening.xlsx
+++ b/Data/SchoolReopening.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akunerth/Dropbox (University of Oregon)/Rapid Response Research (R3)/Data Management R3/EE_R3 Question Bank/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B675C7-FD7E-F540-8934-06C51900069A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95A223F-5A90-E647-8A6C-422F12224BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1620" windowWidth="26840" windowHeight="15540" xr2:uid="{3E9CDE0F-FA6F-034A-9811-7F7D1FC042E9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Question</t>
   </si>
@@ -494,7 +494,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -523,7 +523,9 @@
         <v>4</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
       <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
@@ -535,6 +537,9 @@
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
@@ -546,6 +551,9 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>19</v>
       </c>
@@ -557,6 +565,9 @@
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
@@ -568,6 +579,9 @@
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
@@ -578,6 +592,9 @@
       </c>
       <c r="B7" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>19</v>

</xml_diff>